<commit_message>
Differentiate between const and CV voltage excitation sequence
</commit_message>
<xml_diff>
--- a/Command Set - GUI to MCU.xlsx
+++ b/Command Set - GUI to MCU.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\RWTH-Life\Master\AixSense\DATA team\BioSensor-Readout\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47E1A758-5ADE-4A13-A95D-F627E420EFF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{597C6EB5-4CF4-413C-85F1-CA4D5DC887C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="30960" windowHeight="16800" xr2:uid="{00DEE458-2125-4D3A-B1F7-B3DA3C1D4F9B}"/>
   </bookViews>
   <sheets>
     <sheet name="GUI to MCU" sheetId="1" r:id="rId1"/>
+    <sheet name="MCU to GUI" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="39">
   <si>
     <t>Description</t>
   </si>
@@ -37,12 +38,6 @@
   </si>
   <si>
     <t>Input Parameters</t>
-  </si>
-  <si>
-    <t>Start measurement sequence</t>
-  </si>
-  <si>
-    <t>Starts the measurement sequence programmed in the firmware</t>
   </si>
   <si>
     <t>Stop measurement sequence</t>
@@ -61,19 +56,10 @@
     <t>sub commands :</t>
   </si>
   <si>
-    <t>Set the value of the voltage level</t>
-  </si>
-  <si>
-    <t>Set the value of the measurement duration</t>
-  </si>
-  <si>
     <t>x</t>
   </si>
   <si>
     <t>value (4 bytes)</t>
-  </si>
-  <si>
-    <t>Command ID (dec.)</t>
   </si>
   <si>
     <t>Stops a configuration of parameters</t>
@@ -113,17 +99,80 @@
 0 if cmd ID not recognized</t>
   </si>
   <si>
-    <t>Set Voltage [mV]</t>
-  </si>
-  <si>
-    <t>Set Duration [us]</t>
+    <t>Measurement data</t>
+  </si>
+  <si>
+    <t>To Be Implemented ...</t>
+  </si>
+  <si>
+    <t>Command ID as decimal (1 byte)</t>
+  </si>
+  <si>
+    <t>Config success bool</t>
+  </si>
+  <si>
+    <t>Send return bool whether a parameter was set successfully</t>
+  </si>
+  <si>
+    <t>char buff[] = "0-32132\n";
+in order to send the number 32132</t>
+  </si>
+  <si>
+    <t>Send a single measurement data
+The minus '-' is used as a separator
+The last character is used to mark the end, so a simple serialPort.ReadLine() can be performed</t>
+  </si>
+  <si>
+    <t>char buff[] = "1-1\n";
+to confirm that a parameter was set</t>
+  </si>
+  <si>
+    <t>Command Format ↓</t>
+  </si>
+  <si>
+    <t>char array :
+'ID + '-' + VALUE  + '\n'</t>
+  </si>
+  <si>
+    <t>char array :
+'ID + '-' + boolValue + '\n'</t>
+  </si>
+  <si>
+    <t>Set const excitation Voltage [mV]</t>
+  </si>
+  <si>
+    <t>Set CV excitation Voltage 1 [mV]</t>
+  </si>
+  <si>
+    <t>Set CV excitation Voltage 2 [mV]</t>
+  </si>
+  <si>
+    <t>Set the value of the voltage level for const excitation sequence</t>
+  </si>
+  <si>
+    <t>Set the value of the voltage 2 level for CV excitation sequence</t>
+  </si>
+  <si>
+    <t>Set the value of the voltage 1 level for CV excitation sequence</t>
+  </si>
+  <si>
+    <t>Start const voltage measurement sequence</t>
+  </si>
+  <si>
+    <t>Starts the measurement sequence with const excitation voltage</t>
+  </si>
+  <si>
+    <t>Start CV measurement sequence</t>
+  </si>
+  <si>
+    <t>Starts the measurement sequence with CV excitation voltage</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -183,8 +232,14 @@
       <name val="Bahnschrift Light"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="2"/>
+      <name val="Arial Black"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -210,6 +265,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1" tint="0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -295,7 +356,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -306,28 +367,10 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyAlignment="1">
@@ -359,6 +402,36 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="3" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="60% - Accent3" xfId="3" builtinId="40"/>
@@ -384,15 +457,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>476250</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>1095375</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:colOff>1104900</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -407,8 +480,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="8820150" y="2276475"/>
-          <a:ext cx="619125" cy="1133475"/>
+          <a:off x="8829675" y="3543300"/>
+          <a:ext cx="619125" cy="1323975"/>
         </a:xfrm>
         <a:prstGeom prst="downArrow">
           <a:avLst>
@@ -471,18 +544,18 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>958738</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>9526</xdr:rowOff>
+      <xdr:colOff>968263</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>85726</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>803412</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>43962</xdr:rowOff>
+      <xdr:colOff>812937</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>120162</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2">
@@ -496,8 +569,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="7750477" y="3711852"/>
-              <a:ext cx="2958935" cy="3082436"/>
+              <a:off x="7750063" y="4981576"/>
+              <a:ext cx="2959349" cy="3082436"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -534,7 +607,23 @@
               </a:r>
               <a:r>
                 <a:rPr lang="en-US" sz="1200" b="1" baseline="0"/>
-                <a:t> sub-commands &amp; Input Parameters should be sent separately after the cmd ID,</a:t>
+                <a:t> </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1200" b="1" u="sng" baseline="0"/>
+                <a:t>sub-commands</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1200" b="1" baseline="0"/>
+                <a:t> &amp; </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1200" b="1" u="sng" baseline="0"/>
+                <a:t>Input Parameters</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1200" b="1" baseline="0"/>
+                <a:t> should be sent separately after the cmd ID,</a:t>
               </a:r>
             </a:p>
             <a:p>
@@ -982,7 +1071,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2">
@@ -996,8 +1085,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="7750477" y="3711852"/>
-              <a:ext cx="2958935" cy="3082436"/>
+              <a:off x="7750063" y="4981576"/>
+              <a:ext cx="2959349" cy="3082436"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1034,7 +1123,23 @@
               </a:r>
               <a:r>
                 <a:rPr lang="en-US" sz="1200" b="1" baseline="0"/>
-                <a:t> sub-commands &amp; Input Parameters should be sent separately after the cmd ID,</a:t>
+                <a:t> </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1200" b="1" u="sng" baseline="0"/>
+                <a:t>sub-commands</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1200" b="1" baseline="0"/>
+                <a:t> &amp; </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1200" b="1" u="sng" baseline="0"/>
+                <a:t>Input Parameters</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1200" b="1" baseline="0"/>
+                <a:t> should be sent separately after the cmd ID,</a:t>
               </a:r>
             </a:p>
             <a:p>
@@ -1764,10 +1869,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CA948A5-ACD5-4726-BBD0-3C532A9FE5D2}">
-  <dimension ref="A1:J39"/>
+  <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1777,572 +1882,1146 @@
     <col min="3" max="3" width="62.5703125" style="2" customWidth="1"/>
     <col min="4" max="4" width="9.42578125" style="2" customWidth="1"/>
     <col min="5" max="5" width="23.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="58.28515625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="58.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24" style="2" customWidth="1"/>
+    <col min="7" max="7" width="29.28515625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="58.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="36" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="5"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+    </row>
+    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+    </row>
+    <row r="3" spans="1:10" ht="39" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="5"/>
+      <c r="B3" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="22"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" s="5"/>
+    </row>
+    <row r="4" spans="1:10" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="B4" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="4">
+        <v>1</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" s="5"/>
+    </row>
+    <row r="5" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+      <c r="B5" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="4">
+        <v>2</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J5" s="5"/>
+    </row>
+    <row r="6" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
+      <c r="B6" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="4">
+        <v>0</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J6" s="5"/>
+    </row>
+    <row r="7" spans="1:10" ht="45" x14ac:dyDescent="0.2">
+      <c r="A7" s="5"/>
+      <c r="B7" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="4">
+        <v>5</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="H7" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7" s="8"/>
+    </row>
+    <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="5"/>
+      <c r="B8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="20"/>
+      <c r="E8" s="4">
+        <v>100</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="J8" s="9"/>
+    </row>
+    <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="5"/>
+      <c r="C9" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="20"/>
+      <c r="E9" s="4">
+        <v>101</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="I9" s="6"/>
+      <c r="J9" s="9"/>
+    </row>
+    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+      <c r="C10" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="20"/>
+      <c r="E10" s="4">
+        <v>102</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H10" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="I10" s="6"/>
+      <c r="J10" s="9"/>
+    </row>
+    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="5"/>
+      <c r="C11" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="20"/>
+      <c r="E11" s="4">
+        <v>6</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="I11" s="6"/>
+      <c r="J11" s="5"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="5"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
+      <c r="J27" s="5"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="5"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="5"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
+      <c r="J30" s="5"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="5"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="5"/>
+      <c r="J31" s="5"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="5"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="5"/>
+      <c r="J32" s="5"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="5"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="5"/>
+      <c r="J33" s="5"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="5"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
+      <c r="H34" s="5"/>
+      <c r="I34" s="5"/>
+      <c r="J34" s="5"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="5"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
+      <c r="H35" s="5"/>
+      <c r="I35" s="5"/>
+      <c r="J35" s="5"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="5"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="5"/>
+      <c r="H36" s="5"/>
+      <c r="I36" s="5"/>
+      <c r="J36" s="5"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="5"/>
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="5"/>
+      <c r="H37" s="5"/>
+      <c r="I37" s="5"/>
+      <c r="J37" s="5"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="5"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="5"/>
+      <c r="H38" s="5"/>
+      <c r="I38" s="5"/>
+      <c r="J38" s="5"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="5"/>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="5"/>
+      <c r="H39" s="5"/>
+      <c r="I39" s="5"/>
+      <c r="J39" s="5"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" s="5"/>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
+      <c r="H40" s="5"/>
+      <c r="I40" s="5"/>
+      <c r="J40" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="B5:D5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1A81EA8-1AB3-428B-9C7B-3B8EAD5CE1EF}">
+  <dimension ref="A1:J39"/>
+  <sheetViews>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="2" max="2" width="10.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="37.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="8.140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="23.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="54" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="37.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="6"/>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
+      <c r="A1" s="5"/>
+      <c r="B1" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="26"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-    </row>
-    <row r="3" spans="1:10" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="6"/>
-      <c r="B3" s="8" t="s">
+      <c r="A2" s="5"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+    </row>
+    <row r="3" spans="1:10" ht="39" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="5"/>
+      <c r="B3" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="G3" s="17" t="s">
+      <c r="C3" s="22"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="17" t="s">
+      <c r="H3" s="11" t="s">
         <v>0</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J3" s="6"/>
-    </row>
-    <row r="4" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
-      <c r="B4" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="5">
+        <v>6</v>
+      </c>
+      <c r="J3" s="5"/>
+    </row>
+    <row r="4" spans="1:10" ht="60.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="B4" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="4">
+        <v>0</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4" s="5"/>
+    </row>
+    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+      <c r="B5" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="4">
         <v>1</v>
       </c>
-      <c r="F4" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J4" s="6"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
-      <c r="B5" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="5">
-        <v>0</v>
-      </c>
-      <c r="F5" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J5" s="6"/>
-    </row>
-    <row r="6" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="6"/>
-      <c r="B6" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="5">
-        <v>5</v>
-      </c>
-      <c r="F6" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="H6" s="22" t="s">
+      <c r="F5" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="J6" s="14"/>
-    </row>
-    <row r="7" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="B7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="5">
-        <v>100</v>
-      </c>
-      <c r="F7" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="H7" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="I7" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="J7" s="15"/>
-    </row>
-    <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
-      <c r="C8" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="5">
-        <v>101</v>
-      </c>
-      <c r="F8" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="G8" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="H8" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="I8" s="12"/>
-      <c r="J8" s="15"/>
-    </row>
-    <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
-      <c r="C9" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="5">
-        <v>6</v>
-      </c>
-      <c r="F9" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G9" s="19" t="s">
+      <c r="H5" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="H9" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="I9" s="12"/>
-      <c r="J9" s="6"/>
+      <c r="I5" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="J5" s="5"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="6"/>
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="6"/>
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="6"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="6"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="6"/>
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="6"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="6"/>
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="6"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
-      <c r="J24" s="6"/>
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="6"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
-      <c r="J25" s="6"/>
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="6"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="6"/>
-      <c r="J26" s="6"/>
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="5"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="6"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="6"/>
-      <c r="J27" s="6"/>
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
+      <c r="J27" s="5"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="6"/>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
-      <c r="I28" s="6"/>
-      <c r="J28" s="6"/>
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="5"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="6"/>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
-      <c r="I29" s="6"/>
-      <c r="J29" s="6"/>
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="5"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="6"/>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="6"/>
-      <c r="I30" s="6"/>
-      <c r="J30" s="6"/>
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
+      <c r="J30" s="5"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="6"/>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="6"/>
-      <c r="H31" s="6"/>
-      <c r="I31" s="6"/>
-      <c r="J31" s="6"/>
+      <c r="A31" s="5"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="5"/>
+      <c r="J31" s="5"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="6"/>
-      <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="6"/>
-      <c r="G32" s="6"/>
-      <c r="H32" s="6"/>
-      <c r="I32" s="6"/>
-      <c r="J32" s="6"/>
+      <c r="A32" s="5"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="5"/>
+      <c r="J32" s="5"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="6"/>
-      <c r="B33" s="6"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="6"/>
-      <c r="G33" s="6"/>
-      <c r="H33" s="6"/>
-      <c r="I33" s="6"/>
-      <c r="J33" s="6"/>
+      <c r="A33" s="5"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="5"/>
+      <c r="J33" s="5"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="6"/>
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="6"/>
-      <c r="G34" s="6"/>
-      <c r="H34" s="6"/>
-      <c r="I34" s="6"/>
-      <c r="J34" s="6"/>
+      <c r="A34" s="5"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
+      <c r="H34" s="5"/>
+      <c r="I34" s="5"/>
+      <c r="J34" s="5"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="6"/>
-      <c r="B35" s="6"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="6"/>
-      <c r="E35" s="6"/>
-      <c r="F35" s="6"/>
-      <c r="G35" s="6"/>
-      <c r="H35" s="6"/>
-      <c r="I35" s="6"/>
-      <c r="J35" s="6"/>
+      <c r="A35" s="5"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
+      <c r="H35" s="5"/>
+      <c r="I35" s="5"/>
+      <c r="J35" s="5"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="6"/>
-      <c r="B36" s="6"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="6"/>
-      <c r="G36" s="6"/>
-      <c r="H36" s="6"/>
-      <c r="I36" s="6"/>
-      <c r="J36" s="6"/>
+      <c r="A36" s="5"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="5"/>
+      <c r="H36" s="5"/>
+      <c r="I36" s="5"/>
+      <c r="J36" s="5"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="6"/>
-      <c r="B37" s="6"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="6"/>
-      <c r="G37" s="6"/>
-      <c r="H37" s="6"/>
-      <c r="I37" s="6"/>
-      <c r="J37" s="6"/>
+      <c r="A37" s="5"/>
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="5"/>
+      <c r="H37" s="5"/>
+      <c r="I37" s="5"/>
+      <c r="J37" s="5"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="6"/>
-      <c r="B38" s="6"/>
-      <c r="C38" s="6"/>
-      <c r="D38" s="6"/>
-      <c r="E38" s="6"/>
-      <c r="F38" s="6"/>
-      <c r="G38" s="6"/>
-      <c r="H38" s="6"/>
-      <c r="I38" s="6"/>
-      <c r="J38" s="6"/>
+      <c r="A38" s="5"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="5"/>
+      <c r="H38" s="5"/>
+      <c r="I38" s="5"/>
+      <c r="J38" s="5"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="6"/>
-      <c r="B39" s="6"/>
-      <c r="C39" s="6"/>
-      <c r="D39" s="6"/>
-      <c r="E39" s="6"/>
-      <c r="F39" s="6"/>
-      <c r="G39" s="6"/>
-      <c r="H39" s="6"/>
-      <c r="I39" s="6"/>
-      <c r="J39" s="6"/>
+      <c r="A39" s="5"/>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="5"/>
+      <c r="H39" s="5"/>
+      <c r="I39" s="5"/>
+      <c r="J39" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C8:D8"/>
+  <mergeCells count="4">
+    <mergeCell ref="B1:C2"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="C7:D7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Configurable CV voltage excitation sequence
</commit_message>
<xml_diff>
--- a/Command Set - GUI to MCU.xlsx
+++ b/Command Set - GUI to MCU.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\RWTH-Life\Master\AixSense\DATA team\BioSensor-Readout\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{597C6EB5-4CF4-413C-85F1-CA4D5DC887C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E761E657-8266-4A80-A05B-19A234A24090}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="30960" windowHeight="16800" xr2:uid="{00DEE458-2125-4D3A-B1F7-B3DA3C1D4F9B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00DEE458-2125-4D3A-B1F7-B3DA3C1D4F9B}"/>
   </bookViews>
   <sheets>
     <sheet name="GUI to MCU" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="41">
   <si>
     <t>Description</t>
   </si>
@@ -166,6 +166,12 @@
   </si>
   <si>
     <t>Starts the measurement sequence with CV excitation voltage</t>
+  </si>
+  <si>
+    <t>Set slope duration between Voltage1 &amp; Voltage2 for CV signal [us]</t>
+  </si>
+  <si>
+    <t>Set slope duration between voltage 1 &amp; 2 for the CV signal</t>
   </si>
 </sst>
 </file>
@@ -458,13 +464,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1104900</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -545,13 +551,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>968263</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>85726</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>812937</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>120162</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
@@ -1869,27 +1875,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CA948A5-ACD5-4726-BBD0-3C532A9FE5D2}">
-  <dimension ref="A1:J40"/>
+  <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="20.5703125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="62.5703125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="23.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="2"/>
+    <col min="2" max="2" width="20.5546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="62.5546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="9.44140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="23.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24" style="2" customWidth="1"/>
-    <col min="7" max="7" width="29.28515625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="58.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.33203125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="58.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="36" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="2"/>
+    <col min="10" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="5"/>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -1901,7 +1907,7 @@
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -1913,7 +1919,7 @@
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
     </row>
-    <row r="3" spans="1:10" ht="39" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="37.200000000000003" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="5"/>
       <c r="B3" s="21" t="s">
         <v>1</v>
@@ -1937,7 +1943,7 @@
       </c>
       <c r="J3" s="5"/>
     </row>
-    <row r="4" spans="1:10" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5"/>
       <c r="B4" s="24" t="s">
         <v>35</v>
@@ -1961,7 +1967,7 @@
       </c>
       <c r="J4" s="5"/>
     </row>
-    <row r="5" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5"/>
       <c r="B5" s="24" t="s">
         <v>37</v>
@@ -1985,7 +1991,7 @@
       </c>
       <c r="J5" s="5"/>
     </row>
-    <row r="6" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5"/>
       <c r="B6" s="24" t="s">
         <v>4</v>
@@ -2009,7 +2015,7 @@
       </c>
       <c r="J6" s="5"/>
     </row>
-    <row r="7" spans="1:10" ht="45" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="43.2" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="24" t="s">
         <v>12</v>
@@ -2033,7 +2039,7 @@
       </c>
       <c r="J7" s="8"/>
     </row>
-    <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
       <c r="B8" s="1" t="s">
         <v>8</v>
@@ -2059,7 +2065,7 @@
       </c>
       <c r="J8" s="9"/>
     </row>
-    <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
       <c r="C9" s="20" t="s">
         <v>30</v>
@@ -2080,7 +2086,7 @@
       <c r="I9" s="6"/>
       <c r="J9" s="9"/>
     </row>
-    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
       <c r="C10" s="20" t="s">
         <v>31</v>
@@ -2101,40 +2107,49 @@
       <c r="I10" s="6"/>
       <c r="J10" s="9"/>
     </row>
-    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
       <c r="C11" s="20" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="D11" s="20"/>
       <c r="E11" s="4">
+        <v>103</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="I11" s="6"/>
+      <c r="J11" s="9"/>
+    </row>
+    <row r="12" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="5"/>
+      <c r="C12" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="20"/>
+      <c r="E12" s="4">
         <v>6</v>
       </c>
-      <c r="F11" s="12" t="s">
+      <c r="F12" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G11" s="13" t="s">
+      <c r="G12" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="H11" s="14" t="s">
+      <c r="H12" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="I11" s="6"/>
-      <c r="J11" s="5"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
+      <c r="I12" s="6"/>
       <c r="J12" s="5"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -2146,7 +2161,7 @@
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -2158,7 +2173,7 @@
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -2170,7 +2185,7 @@
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -2182,7 +2197,7 @@
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -2194,7 +2209,7 @@
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -2206,7 +2221,7 @@
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -2218,7 +2233,7 @@
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -2230,7 +2245,7 @@
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -2242,7 +2257,7 @@
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -2254,7 +2269,7 @@
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -2266,7 +2281,7 @@
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
@@ -2278,7 +2293,7 @@
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
@@ -2290,7 +2305,7 @@
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
@@ -2302,7 +2317,7 @@
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
@@ -2314,7 +2329,7 @@
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
@@ -2326,7 +2341,7 @@
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
@@ -2338,7 +2353,7 @@
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
@@ -2350,7 +2365,7 @@
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
@@ -2362,7 +2377,7 @@
       <c r="I31" s="5"/>
       <c r="J31" s="5"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
@@ -2374,7 +2389,7 @@
       <c r="I32" s="5"/>
       <c r="J32" s="5"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
@@ -2386,7 +2401,7 @@
       <c r="I33" s="5"/>
       <c r="J33" s="5"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
@@ -2398,7 +2413,7 @@
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="5"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
@@ -2410,7 +2425,7 @@
       <c r="I35" s="5"/>
       <c r="J35" s="5"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
@@ -2422,7 +2437,7 @@
       <c r="I36" s="5"/>
       <c r="J36" s="5"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="5"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
@@ -2434,7 +2449,7 @@
       <c r="I37" s="5"/>
       <c r="J37" s="5"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="5"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
@@ -2446,7 +2461,7 @@
       <c r="I38" s="5"/>
       <c r="J38" s="5"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="5"/>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
@@ -2458,7 +2473,7 @@
       <c r="I39" s="5"/>
       <c r="J39" s="5"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="5"/>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
@@ -2470,9 +2485,21 @@
       <c r="I40" s="5"/>
       <c r="J40" s="5"/>
     </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A41" s="5"/>
+      <c r="B41" s="5"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="5"/>
+      <c r="H41" s="5"/>
+      <c r="I41" s="5"/>
+      <c r="J41" s="5"/>
+    </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="C11:D11"/>
+  <mergeCells count="10">
+    <mergeCell ref="C12:D12"/>
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="B3:D3"/>
@@ -2481,6 +2508,7 @@
     <mergeCell ref="B7:D7"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="B5:D5"/>
+    <mergeCell ref="C11:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2495,21 +2523,21 @@
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="10.42578125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="37.7109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="8.140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="23.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="2"/>
+    <col min="2" max="2" width="10.44140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="37.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="8.109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="23.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="54" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="37.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="2"/>
+    <col min="9" max="9" width="37.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="5"/>
       <c r="B1" s="25" t="s">
         <v>19</v>
@@ -2523,7 +2551,7 @@
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="5"/>
       <c r="B2" s="26"/>
       <c r="C2" s="26"/>
@@ -2535,7 +2563,7 @@
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
     </row>
-    <row r="3" spans="1:10" ht="39" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="37.200000000000003" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="5"/>
       <c r="B3" s="21" t="s">
         <v>1</v>
@@ -2559,7 +2587,7 @@
       </c>
       <c r="J3" s="5"/>
     </row>
-    <row r="4" spans="1:10" ht="60.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="58.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5"/>
       <c r="B4" s="24" t="s">
         <v>18</v>
@@ -2583,7 +2611,7 @@
       </c>
       <c r="J4" s="5"/>
     </row>
-    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="5"/>
       <c r="B5" s="24" t="s">
         <v>21</v>
@@ -2607,7 +2635,7 @@
       </c>
       <c r="J5" s="5"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -2619,7 +2647,7 @@
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -2631,7 +2659,7 @@
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -2643,7 +2671,7 @@
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -2655,7 +2683,7 @@
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -2667,7 +2695,7 @@
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -2679,7 +2707,7 @@
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -2691,7 +2719,7 @@
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -2703,7 +2731,7 @@
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -2715,7 +2743,7 @@
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -2727,7 +2755,7 @@
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -2739,7 +2767,7 @@
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -2751,7 +2779,7 @@
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -2763,7 +2791,7 @@
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -2775,7 +2803,7 @@
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -2787,7 +2815,7 @@
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -2799,7 +2827,7 @@
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -2811,7 +2839,7 @@
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -2823,7 +2851,7 @@
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
@@ -2835,7 +2863,7 @@
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
@@ -2847,7 +2875,7 @@
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
@@ -2859,7 +2887,7 @@
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
@@ -2871,7 +2899,7 @@
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
@@ -2883,7 +2911,7 @@
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
@@ -2895,7 +2923,7 @@
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
@@ -2907,7 +2935,7 @@
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
@@ -2919,7 +2947,7 @@
       <c r="I31" s="5"/>
       <c r="J31" s="5"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
@@ -2931,7 +2959,7 @@
       <c r="I32" s="5"/>
       <c r="J32" s="5"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
@@ -2943,7 +2971,7 @@
       <c r="I33" s="5"/>
       <c r="J33" s="5"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
@@ -2955,7 +2983,7 @@
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="5"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
@@ -2967,7 +2995,7 @@
       <c r="I35" s="5"/>
       <c r="J35" s="5"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
@@ -2979,7 +3007,7 @@
       <c r="I36" s="5"/>
       <c r="J36" s="5"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="5"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
@@ -2991,7 +3019,7 @@
       <c r="I37" s="5"/>
       <c r="J37" s="5"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="5"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
@@ -3003,7 +3031,7 @@
       <c r="I38" s="5"/>
       <c r="J38" s="5"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="5"/>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>

</xml_diff>

<commit_message>
Define format of data sent to GUI
</commit_message>
<xml_diff>
--- a/Command Set - GUI to MCU.xlsx
+++ b/Command Set - GUI to MCU.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\RWTH-Life\Master\AixSense\DATA team\BioSensor-Readout\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E761E657-8266-4A80-A05B-19A234A24090}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A58897AE-C69A-4E5E-A0B9-67F35068BF7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00DEE458-2125-4D3A-B1F7-B3DA3C1D4F9B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="30960" windowHeight="16800" activeTab="1" xr2:uid="{00DEE458-2125-4D3A-B1F7-B3DA3C1D4F9B}"/>
   </bookViews>
   <sheets>
     <sheet name="GUI to MCU" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="47">
   <si>
     <t>Description</t>
   </si>
@@ -99,12 +99,6 @@
 0 if cmd ID not recognized</t>
   </si>
   <si>
-    <t>Measurement data</t>
-  </si>
-  <si>
-    <t>To Be Implemented ...</t>
-  </si>
-  <si>
     <t>Command ID as decimal (1 byte)</t>
   </si>
   <si>
@@ -114,71 +108,187 @@
     <t>Send return bool whether a parameter was set successfully</t>
   </si>
   <si>
-    <t>char buff[] = "0-32132\n";
+    <t>Command Format ↓</t>
+  </si>
+  <si>
+    <t>Set const excitation Voltage [mV]</t>
+  </si>
+  <si>
+    <t>Set CV excitation Voltage 1 [mV]</t>
+  </si>
+  <si>
+    <t>Set CV excitation Voltage 2 [mV]</t>
+  </si>
+  <si>
+    <t>Set the value of the voltage level for const excitation sequence</t>
+  </si>
+  <si>
+    <t>Set the value of the voltage 2 level for CV excitation sequence</t>
+  </si>
+  <si>
+    <t>Set the value of the voltage 1 level for CV excitation sequence</t>
+  </si>
+  <si>
+    <t>Start const voltage measurement sequence</t>
+  </si>
+  <si>
+    <t>Starts the measurement sequence with const excitation voltage</t>
+  </si>
+  <si>
+    <t>Start CV measurement sequence</t>
+  </si>
+  <si>
+    <t>Starts the measurement sequence with CV excitation voltage</t>
+  </si>
+  <si>
+    <t>Set slope duration between Voltage1 &amp; Voltage2 for CV signal [us]</t>
+  </si>
+  <si>
+    <t>Set slope duration between voltage 1 &amp; 2 for the CV signal</t>
+  </si>
+  <si>
+    <t>Measurement data for CV</t>
+  </si>
+  <si>
+    <t>Measurement data for const. voltage</t>
+  </si>
+  <si>
+    <t>Measurement data for EIS</t>
+  </si>
+  <si>
+    <t>Send a single measurement data
+The colon ':' is used as a separator
+The last character is used to mark the end, so a simple serialPort.ReadLine() can be performed</t>
+  </si>
+  <si>
+    <t>Send a single measurement data
+The colon ':' is used as a separator</t>
+  </si>
+  <si>
+    <t>char buff[] = "1:32132\n";
 in order to send the number 32132</t>
   </si>
   <si>
-    <t>Send a single measurement data
-The minus '-' is used as a separator
-The last character is used to mark the end, so a simple serialPort.ReadLine() can be performed</t>
-  </si>
-  <si>
-    <t>char buff[] = "1-1\n";
+    <t>char buff[] = "2:32132\n";
+in order to send the number 32132</t>
+  </si>
+  <si>
+    <t>char buff[] = "3:1000:12:-100:32:120\n";
+in order to send a frequency of 1kHz, real part of Rcal 12, imaginary of -100, etc.</t>
+  </si>
+  <si>
+    <t>Sends multiple int32 values of measurement data
+The colon ':' is used as a separator
+FREQ is frequency value, Re{Rcal} is the real &amp; Im{Rcal} the imaginary part of Rcal (calibration resistor)</t>
+  </si>
+  <si>
+    <t>char array :
+ID + ':' + VALUE  + '\n'</t>
+  </si>
+  <si>
+    <t>char array :
+ID + ':' + boolValue + '\n'</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">char array :
+ID + ':' + FREQ + ':' + </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Re</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">{Rcal} + ':' + </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Im</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">{Rcal} + ':' + </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Re</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">{Zm} + ':' + </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Im</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{Zm} + '\n'</t>
+    </r>
+  </si>
+  <si>
+    <t>char buff[] = "10:1\n";
 to confirm that a parameter was set</t>
-  </si>
-  <si>
-    <t>Command Format ↓</t>
-  </si>
-  <si>
-    <t>char array :
-'ID + '-' + VALUE  + '\n'</t>
-  </si>
-  <si>
-    <t>char array :
-'ID + '-' + boolValue + '\n'</t>
-  </si>
-  <si>
-    <t>Set const excitation Voltage [mV]</t>
-  </si>
-  <si>
-    <t>Set CV excitation Voltage 1 [mV]</t>
-  </si>
-  <si>
-    <t>Set CV excitation Voltage 2 [mV]</t>
-  </si>
-  <si>
-    <t>Set the value of the voltage level for const excitation sequence</t>
-  </si>
-  <si>
-    <t>Set the value of the voltage 2 level for CV excitation sequence</t>
-  </si>
-  <si>
-    <t>Set the value of the voltage 1 level for CV excitation sequence</t>
-  </si>
-  <si>
-    <t>Start const voltage measurement sequence</t>
-  </si>
-  <si>
-    <t>Starts the measurement sequence with const excitation voltage</t>
-  </si>
-  <si>
-    <t>Start CV measurement sequence</t>
-  </si>
-  <si>
-    <t>Starts the measurement sequence with CV excitation voltage</t>
-  </si>
-  <si>
-    <t>Set slope duration between Voltage1 &amp; Voltage2 for CV signal [us]</t>
-  </si>
-  <si>
-    <t>Set slope duration between voltage 1 &amp; 2 for the CV signal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -238,12 +348,6 @@
       <name val="Bahnschrift Light"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="14"/>
-      <color theme="2"/>
-      <name val="Arial Black"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -276,8 +380,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
       </patternFill>
     </fill>
   </fills>
@@ -356,13 +460,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -417,6 +522,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="3" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -432,15 +540,10 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="60% - Accent3" xfId="3" builtinId="40"/>
+    <cellStyle name="60% - Accent4" xfId="4" builtinId="44"/>
     <cellStyle name="Accent3" xfId="2" builtinId="37"/>
     <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -763,7 +866,7 @@
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
-                <a:t>port.sent( 65000 ); // set the value (2bytes)</a:t>
+                <a:t>port.sent( 65000 ); // set the value (4bytes)</a:t>
               </a:r>
             </a:p>
             <a:p>
@@ -1279,7 +1382,7 @@
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
-                <a:t>port.sent( 65000 ); // set the value (2bytes)</a:t>
+                <a:t>port.sent( 65000 ); // set the value (4bytes)</a:t>
               </a:r>
             </a:p>
             <a:p>
@@ -1573,6 +1676,223 @@
         </xdr:sp>
       </mc:Fallback>
     </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>538369</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>107674</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>985631</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>140804</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Arrow: Down 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4CF86BF7-F630-486F-8DFE-AB9239B2170A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000">
+          <a:off x="4911586" y="3288196"/>
+          <a:ext cx="447262" cy="795130"/>
+        </a:xfrm>
+        <a:prstGeom prst="downArrow">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 33333"/>
+            <a:gd name="adj2" fmla="val 57292"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="accent4">
+                <a:lumMod val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="48000">
+              <a:schemeClr val="accent4">
+                <a:lumMod val="97000"/>
+                <a:lumOff val="3000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="accent4">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>339588</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>107675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>323023</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>8282</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DC115717-AD53-4224-9083-C326F776CEB0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4166153" y="4240697"/>
+          <a:ext cx="2095500" cy="662607"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent4">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100" b="1">
+              <a:latin typeface="+mn-lt"/>
+            </a:rPr>
+            <a:t>Currently not implemented;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr kumimoji="0" lang="de-DE" sz="1100" b="1" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:prstClr val="black"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>only the boolValue is being sent </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr kumimoji="0" lang="de-DE" sz="1100" b="1" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:prstClr val="black"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>(1 or 0)</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="0" lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:prstClr val="black"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uLnTx/>
+            <a:uFillTx/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1877,25 +2197,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CA948A5-ACD5-4726-BBD0-3C532A9FE5D2}">
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="2"/>
-    <col min="2" max="2" width="20.5546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="62.5546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="9.44140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="23.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="2" max="2" width="20.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="62.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="23.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24" style="2" customWidth="1"/>
-    <col min="7" max="7" width="29.33203125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="58.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.28515625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="58.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="36" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.109375" style="2"/>
+    <col min="10" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="5"/>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -1907,7 +2227,7 @@
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -1919,15 +2239,15 @@
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
     </row>
-    <row r="3" spans="1:10" ht="37.200000000000003" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="39" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="22"/>
-      <c r="D3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="24"/>
       <c r="E3" s="17" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F3" s="11" t="s">
         <v>3</v>
@@ -1943,13 +2263,13 @@
       </c>
       <c r="J3" s="5"/>
     </row>
-    <row r="4" spans="1:10" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
-      <c r="B4" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
+      <c r="B4" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
       <c r="E4" s="4">
         <v>1</v>
       </c>
@@ -1960,20 +2280,20 @@
         <v>9</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="J4" s="5"/>
     </row>
-    <row r="5" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
-      <c r="B5" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
+      <c r="B5" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
       <c r="E5" s="4">
         <v>2</v>
       </c>
@@ -1984,20 +2304,20 @@
         <v>9</v>
       </c>
       <c r="H5" s="14" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>9</v>
       </c>
       <c r="J5" s="5"/>
     </row>
-    <row r="6" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
       <c r="E6" s="4">
         <v>0</v>
       </c>
@@ -2015,13 +2335,13 @@
       </c>
       <c r="J6" s="5"/>
     </row>
-    <row r="7" spans="1:10" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A7" s="5"/>
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
       <c r="E7" s="4">
         <v>5</v>
       </c>
@@ -2039,15 +2359,15 @@
       </c>
       <c r="J7" s="8"/>
     </row>
-    <row r="8" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" s="20"/>
+      <c r="C8" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="21"/>
       <c r="E8" s="4">
         <v>100</v>
       </c>
@@ -2058,19 +2378,19 @@
         <v>16</v>
       </c>
       <c r="H8" s="14" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="I8" s="7" t="s">
         <v>15</v>
       </c>
       <c r="J8" s="9"/>
     </row>
-    <row r="9" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
-      <c r="C9" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="20"/>
+      <c r="C9" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="21"/>
       <c r="E9" s="4">
         <v>101</v>
       </c>
@@ -2081,17 +2401,17 @@
         <v>16</v>
       </c>
       <c r="H9" s="14" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="I9" s="6"/>
       <c r="J9" s="9"/>
     </row>
-    <row r="10" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
-      <c r="C10" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" s="20"/>
+      <c r="C10" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="21"/>
       <c r="E10" s="4">
         <v>102</v>
       </c>
@@ -2102,17 +2422,17 @@
         <v>16</v>
       </c>
       <c r="H10" s="14" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="I10" s="6"/>
       <c r="J10" s="9"/>
     </row>
-    <row r="11" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
-      <c r="C11" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" s="20"/>
+      <c r="C11" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="21"/>
       <c r="E11" s="4">
         <v>103</v>
       </c>
@@ -2123,17 +2443,17 @@
         <v>16</v>
       </c>
       <c r="H11" s="14" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="I11" s="6"/>
       <c r="J11" s="9"/>
     </row>
-    <row r="12" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
-      <c r="C12" s="20" t="s">
+      <c r="C12" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="20"/>
+      <c r="D12" s="21"/>
       <c r="E12" s="4">
         <v>6</v>
       </c>
@@ -2149,7 +2469,7 @@
       <c r="I12" s="6"/>
       <c r="J12" s="5"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -2161,7 +2481,7 @@
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -2173,7 +2493,7 @@
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -2185,7 +2505,7 @@
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -2197,7 +2517,7 @@
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -2209,7 +2529,7 @@
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -2221,7 +2541,7 @@
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -2233,7 +2553,7 @@
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -2245,7 +2565,7 @@
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -2257,7 +2577,7 @@
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -2269,7 +2589,7 @@
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -2281,7 +2601,7 @@
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
@@ -2293,7 +2613,7 @@
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
@@ -2305,7 +2625,7 @@
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
@@ -2317,7 +2637,7 @@
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
@@ -2329,7 +2649,7 @@
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
@@ -2341,7 +2661,7 @@
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
@@ -2353,7 +2673,7 @@
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
@@ -2365,7 +2685,7 @@
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
@@ -2377,7 +2697,7 @@
       <c r="I31" s="5"/>
       <c r="J31" s="5"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
@@ -2389,7 +2709,7 @@
       <c r="I32" s="5"/>
       <c r="J32" s="5"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
@@ -2401,7 +2721,7 @@
       <c r="I33" s="5"/>
       <c r="J33" s="5"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
@@ -2413,7 +2733,7 @@
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="5"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
@@ -2425,7 +2745,7 @@
       <c r="I35" s="5"/>
       <c r="J35" s="5"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
@@ -2437,7 +2757,7 @@
       <c r="I36" s="5"/>
       <c r="J36" s="5"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="5"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
@@ -2449,7 +2769,7 @@
       <c r="I37" s="5"/>
       <c r="J37" s="5"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="5"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
@@ -2461,7 +2781,7 @@
       <c r="I38" s="5"/>
       <c r="J38" s="5"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="5"/>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
@@ -2473,7 +2793,7 @@
       <c r="I39" s="5"/>
       <c r="J39" s="5"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="5"/>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
@@ -2485,7 +2805,7 @@
       <c r="I40" s="5"/>
       <c r="J40" s="5"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="5"/>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
@@ -2519,30 +2839,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1A81EA8-1AB3-428B-9C7B-3B8EAD5CE1EF}">
   <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="2"/>
-    <col min="2" max="2" width="10.44140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="37.6640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="8.109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="23.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="2" max="2" width="10.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="37.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="8.140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="23.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="54" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="37.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.109375" style="2"/>
+    <col min="9" max="9" width="37.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5"/>
-      <c r="B1" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" s="26"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
@@ -2551,10 +2869,10 @@
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
@@ -2563,18 +2881,18 @@
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
     </row>
-    <row r="3" spans="1:10" ht="37.200000000000003" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="39" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="22"/>
-      <c r="D3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="24"/>
       <c r="E3" s="17" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="G3" s="11" t="s">
         <v>2</v>
@@ -2587,79 +2905,103 @@
       </c>
       <c r="J3" s="5"/>
     </row>
-    <row r="4" spans="1:10" ht="58.2" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="60.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
-      <c r="B4" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
+      <c r="B4" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
       <c r="E4" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4" s="19" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="G4" s="12" t="s">
         <v>9</v>
       </c>
       <c r="H4" s="16" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="I4" s="18" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="J4" s="5"/>
     </row>
-    <row r="5" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
-      <c r="B5" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
+      <c r="B5" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
       <c r="E5" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="G5" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="14" t="s">
-        <v>22</v>
+      <c r="H5" s="16" t="s">
+        <v>38</v>
       </c>
       <c r="I5" s="18" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="J5" s="5"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
+      <c r="B6" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="4">
+        <v>3</v>
+      </c>
+      <c r="F6" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="I6" s="18" t="s">
+        <v>41</v>
+      </c>
       <c r="J6" s="5"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
+      <c r="B7" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="20">
+        <v>10</v>
+      </c>
+      <c r="F7" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="H7" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7" s="18" t="s">
+        <v>46</v>
+      </c>
       <c r="J7" s="5"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -2671,7 +3013,7 @@
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -2683,7 +3025,7 @@
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -2695,7 +3037,7 @@
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -2707,7 +3049,7 @@
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -2719,7 +3061,7 @@
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -2731,7 +3073,7 @@
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -2743,7 +3085,7 @@
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -2755,7 +3097,7 @@
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -2767,7 +3109,7 @@
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -2779,7 +3121,7 @@
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -2791,7 +3133,7 @@
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -2803,7 +3145,7 @@
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -2815,7 +3157,7 @@
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -2827,7 +3169,7 @@
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -2839,7 +3181,7 @@
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -2851,7 +3193,7 @@
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
@@ -2863,7 +3205,7 @@
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
@@ -2875,7 +3217,7 @@
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
@@ -2887,7 +3229,7 @@
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
@@ -2899,7 +3241,7 @@
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
@@ -2911,7 +3253,7 @@
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
@@ -2923,7 +3265,7 @@
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
@@ -2935,7 +3277,7 @@
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
@@ -2947,7 +3289,7 @@
       <c r="I31" s="5"/>
       <c r="J31" s="5"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
@@ -2959,7 +3301,7 @@
       <c r="I32" s="5"/>
       <c r="J32" s="5"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
@@ -2971,7 +3313,7 @@
       <c r="I33" s="5"/>
       <c r="J33" s="5"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
@@ -2983,7 +3325,7 @@
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="5"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
@@ -2995,7 +3337,7 @@
       <c r="I35" s="5"/>
       <c r="J35" s="5"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
@@ -3007,7 +3349,7 @@
       <c r="I36" s="5"/>
       <c r="J36" s="5"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="5"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
@@ -3019,7 +3361,7 @@
       <c r="I37" s="5"/>
       <c r="J37" s="5"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="5"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
@@ -3031,7 +3373,7 @@
       <c r="I38" s="5"/>
       <c r="J38" s="5"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="5"/>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
@@ -3044,12 +3386,14 @@
       <c r="J39" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B1:C2"/>
+  <mergeCells count="5">
+    <mergeCell ref="B7:D7"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B6:D6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update cmd set table & add helper script for sequencer
</commit_message>
<xml_diff>
--- a/Command Set - GUI to MCU.xlsx
+++ b/Command Set - GUI to MCU.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\RWTH-Life\Master\AixSense\DATA team\BioSensor-Readout\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A58897AE-C69A-4E5E-A0B9-67F35068BF7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{017F3D9F-1A66-45D3-9BEA-8928843BCE0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="30960" windowHeight="16800" activeTab="1" xr2:uid="{00DEE458-2125-4D3A-B1F7-B3DA3C1D4F9B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="30960" windowHeight="16800" xr2:uid="{00DEE458-2125-4D3A-B1F7-B3DA3C1D4F9B}"/>
   </bookViews>
   <sheets>
     <sheet name="GUI to MCU" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="54">
   <si>
     <t>Description</t>
   </si>
@@ -282,6 +282,48 @@
   <si>
     <t>char buff[] = "10:1\n";
 to confirm that a parameter was set</t>
+  </si>
+  <si>
+    <t>Set voltage for EIS [mV]</t>
+  </si>
+  <si>
+    <t>Set voltage peak for the AC sinusoidal signal used for EIS</t>
+  </si>
+  <si>
+    <t>Set number of frequencies for EIS (int)</t>
+  </si>
+  <si>
+    <t>Set the number of frequencies used in EIS as an integer
+and the individual frequencies afterwards</t>
+  </si>
+  <si>
+    <t>value (4 bytes)
++ frequencies[] (4*value bytes)</t>
+  </si>
+  <si>
+    <t>define an arbitrary frequency array, e.g. freq[] = {100, 500, 1000}
+port.sent( 107 );
+port.sent( 3 ); // set value (num. of freq.)
+port.sent( 100 );
+port.sent( 500 );
+port.sent( 1000 );</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">success bool (1 byte):
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0 if failed</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -566,15 +608,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>1104900</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:colOff>1123950</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -589,8 +631,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="8829675" y="3543300"/>
-          <a:ext cx="619125" cy="1323975"/>
+          <a:off x="8848725" y="5362575"/>
+          <a:ext cx="619125" cy="1704975"/>
         </a:xfrm>
         <a:prstGeom prst="downArrow">
           <a:avLst>
@@ -653,15 +695,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>968263</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>85726</xdr:rowOff>
+      <xdr:colOff>987313</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>9526</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>812937</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>120162</xdr:rowOff>
+      <xdr:colOff>831987</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>43962</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
       <mc:Choice Requires="a14">
@@ -678,8 +720,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="7750063" y="4981576"/>
-              <a:ext cx="2959349" cy="3082436"/>
+              <a:off x="7769113" y="7181851"/>
+              <a:ext cx="3006974" cy="3082436"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1194,8 +1236,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="7750063" y="4981576"/>
-              <a:ext cx="2959349" cy="3082436"/>
+              <a:off x="7769113" y="7181851"/>
+              <a:ext cx="3006974" cy="3082436"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -2197,8 +2239,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CA948A5-ACD5-4726-BBD0-3C532A9FE5D2}">
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2208,7 +2250,7 @@
     <col min="3" max="3" width="62.5703125" style="2" customWidth="1"/>
     <col min="4" max="4" width="9.42578125" style="2" customWidth="1"/>
     <col min="5" max="5" width="23.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24" style="2" customWidth="1"/>
+    <col min="6" max="6" width="33.7109375" style="2" customWidth="1"/>
     <col min="7" max="7" width="29.28515625" style="2" customWidth="1"/>
     <col min="8" max="8" width="58.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="36" style="2" bestFit="1" customWidth="1"/>
@@ -2451,46 +2493,66 @@
     <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="C12" s="21" t="s">
-        <v>13</v>
+        <v>47</v>
       </c>
       <c r="D12" s="21"/>
       <c r="E12" s="4">
-        <v>6</v>
+        <v>104</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="G12" s="13" t="s">
-        <v>17</v>
+        <v>10</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>16</v>
       </c>
       <c r="H12" s="14" t="s">
-        <v>11</v>
+        <v>48</v>
       </c>
       <c r="I12" s="6"/>
       <c r="J12" s="5"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
+      <c r="C13" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="21"/>
+      <c r="E13" s="4">
+        <v>107</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="H13" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="I13" s="18" t="s">
+        <v>52</v>
+      </c>
       <c r="J13" s="5"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
+      <c r="C14" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="21"/>
+      <c r="E14" s="4">
+        <v>6</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="H14" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="I14" s="6"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -2818,8 +2880,8 @@
       <c r="J41" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="C12:D12"/>
+  <mergeCells count="12">
+    <mergeCell ref="C14:D14"/>
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="B3:D3"/>
@@ -2829,6 +2891,8 @@
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2839,7 +2903,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1A81EA8-1AB3-428B-9C7B-3B8EAD5CE1EF}">
   <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update command set table
</commit_message>
<xml_diff>
--- a/Command Set - GUI to MCU.xlsx
+++ b/Command Set - GUI to MCU.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\RWTH-Life\Master\AixSense\DATA team\BioSensor-Readout\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{017F3D9F-1A66-45D3-9BEA-8928843BCE0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69F069FF-596D-48CD-BDA0-D70D1BA61099}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="30960" windowHeight="16800" xr2:uid="{00DEE458-2125-4D3A-B1F7-B3DA3C1D4F9B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00DEE458-2125-4D3A-B1F7-B3DA3C1D4F9B}"/>
   </bookViews>
   <sheets>
     <sheet name="GUI to MCU" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="56">
   <si>
     <t>Description</t>
   </si>
@@ -324,6 +324,12 @@
       </rPr>
       <t>0 if failed</t>
     </r>
+  </si>
+  <si>
+    <t>Start EIS measurement sequence</t>
+  </si>
+  <si>
+    <t>Starts the EIS measurement sequence (AC sinus. excitation voltage)</t>
   </si>
 </sst>
 </file>
@@ -509,7 +515,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -570,6 +576,9 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -608,15 +617,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>504825</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:colOff>504824</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>141514</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>1123950</xdr:colOff>
+      <xdr:colOff>1123949</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:rowOff>85724</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -631,8 +640,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="8848725" y="5362575"/>
-          <a:ext cx="619125" cy="1704975"/>
+          <a:off x="9093653" y="6564085"/>
+          <a:ext cx="619125" cy="1424668"/>
         </a:xfrm>
         <a:prstGeom prst="downArrow">
           <a:avLst>
@@ -2239,25 +2248,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CA948A5-ACD5-4726-BBD0-3C532A9FE5D2}">
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="20.5703125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="62.5703125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="23.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.7109375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="29.28515625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="58.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="2"/>
+    <col min="2" max="2" width="20.5546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="62.5546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="9.44140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="23.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.6640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="29.33203125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="58.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="36" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="2"/>
+    <col min="10" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="5"/>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -2269,7 +2278,7 @@
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -2281,13 +2290,13 @@
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
     </row>
-    <row r="3" spans="1:10" ht="39" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="37.200000000000003" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="5"/>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="23"/>
-      <c r="D3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="25"/>
       <c r="E3" s="17" t="s">
         <v>18</v>
       </c>
@@ -2305,13 +2314,13 @@
       </c>
       <c r="J3" s="5"/>
     </row>
-    <row r="4" spans="1:10" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5"/>
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
       <c r="E4" s="4">
         <v>1</v>
       </c>
@@ -2329,13 +2338,13 @@
       </c>
       <c r="J4" s="5"/>
     </row>
-    <row r="5" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5"/>
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
       <c r="E5" s="4">
         <v>2</v>
       </c>
@@ -2353,15 +2362,15 @@
       </c>
       <c r="J5" s="5"/>
     </row>
-    <row r="6" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5"/>
-      <c r="B6" s="25" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
+      <c r="B6" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
       <c r="E6" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F6" s="12" t="s">
         <v>9</v>
@@ -2370,92 +2379,95 @@
         <v>9</v>
       </c>
       <c r="H6" s="14" t="s">
-        <v>5</v>
+        <v>55</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="J6" s="5"/>
     </row>
-    <row r="7" spans="1:10" ht="45" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5"/>
-      <c r="B7" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
+      <c r="B7" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
       <c r="E7" s="4">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F7" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G7" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="16" t="s">
+      <c r="H7" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J7" s="5"/>
+    </row>
+    <row r="8" spans="1:10" ht="43.2" x14ac:dyDescent="0.25">
+      <c r="A8" s="5"/>
+      <c r="B8" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="4">
+        <v>5</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="6" t="s">
+      <c r="I8" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="J7" s="8"/>
-    </row>
-    <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="1" t="s">
+      <c r="J8" s="8"/>
+    </row>
+    <row r="9" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="5"/>
+      <c r="B9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="C9" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="21"/>
-      <c r="E8" s="4">
+      <c r="D9" s="22"/>
+      <c r="E9" s="4">
         <v>100</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="H8" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="I8" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="J8" s="9"/>
-    </row>
-    <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="C9" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="21"/>
-      <c r="E9" s="4">
-        <v>101</v>
       </c>
       <c r="F9" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="10" t="s">
+      <c r="G9" s="15" t="s">
         <v>16</v>
       </c>
       <c r="H9" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="I9" s="6"/>
+        <v>25</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>15</v>
+      </c>
       <c r="J9" s="9"/>
     </row>
-    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
       <c r="C10" s="21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D10" s="21"/>
       <c r="E10" s="4">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F10" s="12" t="s">
         <v>10</v>
@@ -2464,19 +2476,19 @@
         <v>16</v>
       </c>
       <c r="H10" s="14" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I10" s="6"/>
       <c r="J10" s="9"/>
     </row>
-    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
       <c r="C11" s="21" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D11" s="21"/>
       <c r="E11" s="4">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F11" s="12" t="s">
         <v>10</v>
@@ -2485,19 +2497,19 @@
         <v>16</v>
       </c>
       <c r="H11" s="14" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="I11" s="6"/>
       <c r="J11" s="9"/>
     </row>
-    <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="C12" s="21" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="D12" s="21"/>
       <c r="E12" s="4">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F12" s="12" t="s">
         <v>10</v>
@@ -2506,68 +2518,77 @@
         <v>16</v>
       </c>
       <c r="H12" s="14" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="I12" s="6"/>
       <c r="J12" s="5"/>
     </row>
-    <row r="13" spans="1:10" ht="120" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
       <c r="C13" s="21" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D13" s="21"/>
       <c r="E13" s="4">
-        <v>107</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>51</v>
+        <v>104</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>10</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="H13" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="I13" s="18" t="s">
-        <v>52</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="H13" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="I13" s="6"/>
       <c r="J13" s="5"/>
     </row>
-    <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A14" s="5"/>
       <c r="C14" s="21" t="s">
-        <v>13</v>
+        <v>49</v>
       </c>
       <c r="D14" s="21"/>
       <c r="E14" s="4">
+        <v>107</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="H14" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="I14" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="J14" s="5"/>
+    </row>
+    <row r="15" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="5"/>
+      <c r="C15" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="21"/>
+      <c r="E15" s="4">
         <v>6</v>
       </c>
-      <c r="F14" s="12" t="s">
+      <c r="F15" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G14" s="13" t="s">
+      <c r="G15" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="H14" s="14" t="s">
+      <c r="H15" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="I14" s="6"/>
-      <c r="J14" s="5"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
+      <c r="I15" s="6"/>
       <c r="J15" s="5"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -2579,7 +2600,7 @@
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -2591,7 +2612,7 @@
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -2603,7 +2624,7 @@
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -2615,7 +2636,7 @@
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -2627,7 +2648,7 @@
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -2639,7 +2660,7 @@
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -2651,7 +2672,7 @@
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -2663,7 +2684,7 @@
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
@@ -2675,7 +2696,7 @@
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
@@ -2687,7 +2708,7 @@
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
@@ -2699,7 +2720,7 @@
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
@@ -2711,7 +2732,7 @@
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
@@ -2723,7 +2744,7 @@
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
@@ -2735,7 +2756,7 @@
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
@@ -2747,7 +2768,7 @@
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
@@ -2759,7 +2780,7 @@
       <c r="I31" s="5"/>
       <c r="J31" s="5"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
@@ -2771,7 +2792,7 @@
       <c r="I32" s="5"/>
       <c r="J32" s="5"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
@@ -2783,7 +2804,7 @@
       <c r="I33" s="5"/>
       <c r="J33" s="5"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
@@ -2795,7 +2816,7 @@
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="5"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
@@ -2807,7 +2828,7 @@
       <c r="I35" s="5"/>
       <c r="J35" s="5"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
@@ -2819,7 +2840,7 @@
       <c r="I36" s="5"/>
       <c r="J36" s="5"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="5"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
@@ -2831,7 +2852,7 @@
       <c r="I37" s="5"/>
       <c r="J37" s="5"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="5"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
@@ -2843,7 +2864,7 @@
       <c r="I38" s="5"/>
       <c r="J38" s="5"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="5"/>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
@@ -2855,7 +2876,7 @@
       <c r="I39" s="5"/>
       <c r="J39" s="5"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="5"/>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
@@ -2867,7 +2888,7 @@
       <c r="I40" s="5"/>
       <c r="J40" s="5"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="5"/>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
@@ -2880,19 +2901,14 @@
       <c r="J41" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C10:D10"/>
+  <mergeCells count="7">
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="B6:D6"/>
     <mergeCell ref="B7:D7"/>
-    <mergeCell ref="C8:D8"/>
     <mergeCell ref="B5:D5"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="B8:D8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2907,21 +2923,21 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="10.42578125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="37.7109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="8.140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="23.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="2"/>
+    <col min="2" max="2" width="10.44140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="37.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="8.109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="23.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="54" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="37.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="2"/>
+    <col min="9" max="9" width="37.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5"/>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -2933,7 +2949,7 @@
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -2945,13 +2961,13 @@
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
     </row>
-    <row r="3" spans="1:10" ht="39" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="37.200000000000003" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="5"/>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="23"/>
-      <c r="D3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="25"/>
       <c r="E3" s="17" t="s">
         <v>18</v>
       </c>
@@ -2969,13 +2985,13 @@
       </c>
       <c r="J3" s="5"/>
     </row>
-    <row r="4" spans="1:10" ht="60.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="58.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5"/>
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
       <c r="E4" s="4">
         <v>1</v>
       </c>
@@ -2993,13 +3009,13 @@
       </c>
       <c r="J4" s="5"/>
     </row>
-    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="5"/>
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
       <c r="E5" s="4">
         <v>2</v>
       </c>
@@ -3017,13 +3033,13 @@
       </c>
       <c r="J5" s="5"/>
     </row>
-    <row r="6" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="5"/>
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
       <c r="E6" s="4">
         <v>3</v>
       </c>
@@ -3041,13 +3057,13 @@
       </c>
       <c r="J6" s="5"/>
     </row>
-    <row r="7" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="5"/>
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
       <c r="E7" s="20">
         <v>10</v>
       </c>
@@ -3065,7 +3081,7 @@
       </c>
       <c r="J7" s="5"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -3077,7 +3093,7 @@
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -3089,7 +3105,7 @@
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -3101,7 +3117,7 @@
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -3113,7 +3129,7 @@
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -3125,7 +3141,7 @@
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -3137,7 +3153,7 @@
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -3149,7 +3165,7 @@
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -3161,7 +3177,7 @@
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -3173,7 +3189,7 @@
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -3185,7 +3201,7 @@
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -3197,7 +3213,7 @@
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -3209,7 +3225,7 @@
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -3221,7 +3237,7 @@
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -3233,7 +3249,7 @@
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -3245,7 +3261,7 @@
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -3257,7 +3273,7 @@
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
@@ -3269,7 +3285,7 @@
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
@@ -3281,7 +3297,7 @@
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
@@ -3293,7 +3309,7 @@
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
@@ -3305,7 +3321,7 @@
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
@@ -3317,7 +3333,7 @@
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
@@ -3329,7 +3345,7 @@
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
@@ -3341,7 +3357,7 @@
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
@@ -3353,7 +3369,7 @@
       <c r="I31" s="5"/>
       <c r="J31" s="5"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
@@ -3365,7 +3381,7 @@
       <c r="I32" s="5"/>
       <c r="J32" s="5"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
@@ -3377,7 +3393,7 @@
       <c r="I33" s="5"/>
       <c r="J33" s="5"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
@@ -3389,7 +3405,7 @@
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="5"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
@@ -3401,7 +3417,7 @@
       <c r="I35" s="5"/>
       <c r="J35" s="5"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
@@ -3413,7 +3429,7 @@
       <c r="I36" s="5"/>
       <c r="J36" s="5"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="5"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
@@ -3425,7 +3441,7 @@
       <c r="I37" s="5"/>
       <c r="J37" s="5"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="5"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
@@ -3437,7 +3453,7 @@
       <c r="I38" s="5"/>
       <c r="J38" s="5"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="5"/>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>

</xml_diff>